<commit_message>
added location for BL trials
</commit_message>
<xml_diff>
--- a/StimuliTable-Encoding-3run-40-discrete-8-12345.xlsx
+++ b/StimuliTable-Encoding-3run-40-discrete-8-12345.xlsx
@@ -1387,10 +1387,10 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K22">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2293,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="J43">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K43">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3199,10 +3199,10 @@
         <v>1</v>
       </c>
       <c r="J64">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K64">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -4105,10 +4105,10 @@
         <v>1</v>
       </c>
       <c r="J85">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K85">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -5011,10 +5011,10 @@
         <v>2</v>
       </c>
       <c r="J106">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K106">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="107" spans="1:17">
@@ -5917,10 +5917,10 @@
         <v>2</v>
       </c>
       <c r="J127">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K127">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="128" spans="1:17">
@@ -6823,10 +6823,10 @@
         <v>2</v>
       </c>
       <c r="J148">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K148">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="149" spans="1:17">
@@ -7729,10 +7729,10 @@
         <v>2</v>
       </c>
       <c r="J169">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K169">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="170" spans="1:17">
@@ -8635,10 +8635,10 @@
         <v>3</v>
       </c>
       <c r="J190">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K190">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="191" spans="1:17">
@@ -9541,10 +9541,10 @@
         <v>3</v>
       </c>
       <c r="J211">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K211">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="212" spans="1:17">
@@ -10447,10 +10447,10 @@
         <v>3</v>
       </c>
       <c r="J232">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K232">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
     <row r="233" spans="1:17">
@@ -11353,10 +11353,10 @@
         <v>3</v>
       </c>
       <c r="J253">
-        <v>259.8076211</v>
+        <v>212.1320344</v>
       </c>
       <c r="K253">
-        <v>150</v>
+        <v>212.1320344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>